<commit_message>
Updated databases, updated tests, updated GUI
</commit_message>
<xml_diff>
--- a/Inventory_Management/Lucy/savedInventory_RoomTemperature.xlsx
+++ b/Inventory_Management/Lucy/savedInventory_RoomTemperature.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Description</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>Viagra</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -182,28 +185,63 @@
         <v>15</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>1234.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>16</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>20.0</v>
+        <v>22.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>21.0</v>
+        <v>23.0</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>100.0</v>
+        <v>986.52</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>10.0</v>
+        <v>23.62</v>
       </c>
       <c r="H2" t="n" s="0">
         <v>1000.0</v>
       </c>
       <c r="I2" t="n" s="0">
         <v>100.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>1234.0</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>22.0</v>
+      </c>
+      <c r="J3" t="n" s="0">
+        <v>1000.0</v>
+      </c>
+      <c r="K3" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="L3" t="n" s="0">
+        <v>91.0</v>
+      </c>
+      <c r="M3" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="N3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O3" t="n" s="0">
+        <v>20.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>